<commit_message>
Fix DB Save Vendings
</commit_message>
<xml_diff>
--- a/projects/Nazarov/ControlWork_Preview/ControlWork_Preview/Resources/Excel.xlsx
+++ b/projects/Nazarov/ControlWork_Preview/ControlWork_Preview/Resources/Excel.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Название</t>
   </si>
@@ -85,16 +85,46 @@
     <t>2</t>
   </si>
   <si>
-    <t>Opera</t>
-  </si>
-  <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>213</t>
+    <t>Opel</t>
+  </si>
+  <si>
+    <t>1243</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
   <si>
     <t>France</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Opera__XAML__</t>
+  </si>
+  <si>
+    <t>4312</t>
+  </si>
+  <si>
+    <t>4123</t>
+  </si>
+  <si>
+    <t>g53</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>OPLA</t>
+  </si>
+  <si>
+    <t>1423</t>
+  </si>
+  <si>
+    <t>312</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
@@ -709,7 +739,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -766,6 +796,40 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>